<commit_message>
fix: troca planilha modelo
</commit_message>
<xml_diff>
--- a/public/assets/modelo-pix.xlsx
+++ b/public/assets/modelo-pix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vcaconstrutora781-my.sharepoint.com/personal/otavio_nascimento_vcaconstrutora_com_br/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{A7D83A30-720F-4397-B7B1-8080EA8E9554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08BD74A9-551F-44BF-BAA2-193561896576}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="8_{A7D83A30-720F-4397-B7B1-8080EA8E9554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1ED3ACD3-5568-4939-B6B9-3EF88C13056C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A63FF177-2295-4600-A292-FB9CE2200153}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Chave Pix</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Escolha uma das opções da lista: Celular/Telefone, CPF/CNPJ, E-mail, Outro</t>
+  </si>
+  <si>
+    <t>Limite de 25 caracteres e sem espaços em branco</t>
   </si>
 </sst>
 </file>
@@ -544,6 +547,7 @@
     <col min="4" max="4" width="25.88671875" style="7" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" style="8" customWidth="1"/>
     <col min="6" max="6" width="47.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -583,12 +587,11 @@
       <formula1>1</formula1>
       <formula2>25</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="O identificador precisa ter até 25 caracteres." sqref="F2:F1048576" xr:uid="{640AA708-0480-4432-9CAC-EB220287FE36}">
-      <formula1>1</formula1>
-      <formula2>25</formula2>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{ADBD9F08-B35C-426D-9104-1AD73A8948EA}">
       <formula1>"Celular/Telefone, CPF/CNPJ, E-mail, Outro"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="O identificador precisa ter até 25 caracteres e sem espaços em branco." sqref="F2:F1048576" xr:uid="{CF614FE6-DB7D-482C-AB8A-5F2744C84331}">
+      <formula1>AND(LEN(F2)&gt;=1,LEN(F2)&lt;=25,ISERROR(FIND(" ",F2)))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -599,9 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097F4CFB-3D85-47CF-A6B7-6AEA4E31F0E1}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -654,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>